<commit_message>
updated ICDC study obj ids 09/02
</commit_message>
<xml_diff>
--- a/InputFiles/TC42_Canine_Filter_Breed-ShihTzu.xlsx
+++ b/InputFiles/TC42_Canine_Filter_Breed-ShihTzu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82131028-199B-4C58-B44A-4F118BECB434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAC7A6B-DABD-4EDA-AF4A-0A2116DCBA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 MATCH (c)&lt;--(diag:diagnosis)
 OPTIONAL MATCH (samp:sample)--&gt;(c)
 OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
 RETURN  
        coalesce(c.case_id, '') AS `Case ID`,
        coalesce(s.clinical_study_designation, '') AS `Study Code`,
@@ -550,20 +550,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" customWidth="1"/>
-    <col min="2" max="2" width="92.453125" customWidth="1"/>
-    <col min="3" max="3" width="86.26953125" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="92.42578125" customWidth="1"/>
+    <col min="3" max="3" width="86.28515625" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -580,7 +580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -597,7 +597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -614,7 +614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -631,7 +631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -648,28 +648,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
     </row>
   </sheetData>
@@ -685,7 +685,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>